<commit_message>
virtual participation of cf round 757
</commit_message>
<xml_diff>
--- a/codeforces/problem_journal.xlsx
+++ b/codeforces/problem_journal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d29575c5b92d780/Ace_to_a_TopCoder/competitive-programming/codeforces/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charles/OneDrive/Ace_to_a_TopCoder/competitive-programming/codeforces/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="13_ncr:40009_{1E001B8B-697E-D141-A969-39B7242A4487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36CC9362-E024-2546-B6AE-0B2A14E7860B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2459E60B-7E5C-9F4A-8B13-FD6F41E836BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="500" windowWidth="42140" windowHeight="26420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="199">
   <si>
     <t>Problem</t>
   </si>
@@ -521,6 +521,102 @@
   </si>
   <si>
     <t>Use number theory to find the pattern of a,b,c. Then find the number of odd numbers in it.</t>
+  </si>
+  <si>
+    <t>1611b</t>
+  </si>
+  <si>
+    <t>1611c</t>
+  </si>
+  <si>
+    <t>Given a, b, as numbers of programmers and mathematicians, each team has 4 people and we must mix them. Find the maximum number of teams.</t>
+  </si>
+  <si>
+    <t>Using (a+b)/4 to find the maximum number of teams without the constraint. Then min(a, b, (a+b)/4) should be the answer, because we must include them together.</t>
+  </si>
+  <si>
+    <t>1611d</t>
+  </si>
+  <si>
+    <t>This one is a bit tricky, because we always choose the smaller one, so we can put the larget one at one end.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given an array, each time we pick the smaller one of the left end and right end, put it to a new array, at the left if it's from the left and right if it's from the right. Out put an array to generate the given array. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given a tree with n vertices, assign weights to edges, such that given a sequence order p, the weights to the root is following that order. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The key is d[p[i]] &lt; d[p[i+1]]. The tree structure is given. We maintain a distance array for the nodes. We know d[root] = 0, then when we see a p[i], we check if it's father has been visited and check d[father]. We make the weights to the top to be just i, so the assigned weight from p[i] to its father is just i-d[father]. Done.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I made a mistake. I thought when we see a p[i], we need to update all its ancestors, but we just need to check it's father's weight and whether it's father has been visited. Because if one of its ancestors wasn't visited, this unvisited one's direct child will find it before the current one finds it. Maintaining that array d can make sure that we don't miss one ancestor. </t>
+  </si>
+  <si>
+    <t>1612b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given an even number n, and a number a, b. Output a permutation such that a is the smallest on the left half and b is the largest on the right half. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note that we just need to check if we have enough numbers for a and b to fill in, then the problem can be solved, it's not difficult at all. </t>
+  </si>
+  <si>
+    <t>1612c</t>
+  </si>
+  <si>
+    <t>binary search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given k,x, you try to output 1,2,3…,k-1,k,k-1,k-2,…,1 messages. If the sum exceeds x, you get banned. Out put the maximum number of messages you can go. </t>
+  </si>
+  <si>
+    <t>vairants of binary search can be converted to binary search</t>
+  </si>
+  <si>
+    <t>1612d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The trick is to compute the (yes no) for mid in a clever way, then that is our binary search. </t>
+  </si>
+  <si>
+    <t>The first time I do this question, I used binary search in a redundant way, I split the array to two parts then do it, this increases the difficulty. I also made a stupid mistake when I passed k to the function g.</t>
+  </si>
+  <si>
+    <t>Given a,b, replace a or b by |a-b|. If x can be obtained by this operation, then we out put YES, else NO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Got TLE during the contest. I was stupid, I let a,b do the operations, but I should just realize that if x is not in [min, max], then replace max to max % min. </t>
+  </si>
+  <si>
+    <t>Note that if a &gt; b, then they will be replaced by a-b, b, until the number is smaller than b, then this continues. Hence when we can reach x, it means that x &gt; min(a,b) and (max-x)%min = 0. Otherwise, replace the max by max % min, to save time, until one of them becomes 0.</t>
+  </si>
+  <si>
+    <t>1614b</t>
+  </si>
+  <si>
+    <t>1614c</t>
+  </si>
+  <si>
+    <t>Given number of visits, arrange locations to make the total time minimized.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The problem is easy to solve. </t>
+  </si>
+  <si>
+    <t>I made a mistake when using map, I fogot there might be duplicated keys.</t>
+  </si>
+  <si>
+    <t>map&lt; ll,ll, greater&lt;ll&gt; &gt;, sort(begin,end, f) where f is just a function to compare things in the container.</t>
+  </si>
+  <si>
+    <t>fastpower, while pow is not zero, do it from base.</t>
+  </si>
+  <si>
+    <t>Given OR of intervals in an array, output the sum of XORs of all subsequence. Given n numbers, and m ORs.</t>
+  </si>
+  <si>
+    <t>The problem is tricky. As long as we find the answer is just m * 2^{n-1} we are done, note that we can speed up by using fast power. We just use m to detect total position of 1s.</t>
   </si>
 </sst>
 </file>
@@ -1007,16 +1103,16 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1373,764 +1469,907 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="32.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="49.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.83203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="36" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="29.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="36" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>1600</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>1100</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" ht="136" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>1600</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>1200</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>1500</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>1900</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="G7" s="1"/>
+      <c r="H7" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>1200</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="1"/>
+      <c r="H8" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:8" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>1100</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>1500</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>800</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
+      <c r="G11" s="1"/>
+      <c r="H11" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:8" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>1000</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>1300</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
+      <c r="G13" s="1"/>
+      <c r="H13" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:8" s="2" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>1600</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>1200</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
+      <c r="G15" s="1"/>
+      <c r="H15" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:8" s="2" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>1400</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:8" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>900</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="3" customFormat="1" ht="187" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:8" s="2" customFormat="1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>1700</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
+      <c r="G18" s="1"/>
+      <c r="H18" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="3" customFormat="1" ht="221" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:8" s="2" customFormat="1" ht="221" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>1900</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:8" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>900</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2" t="s">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
+      <c r="G20" s="1"/>
+      <c r="H20" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:8" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>1700</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="G21" s="1"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>1100</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2" t="s">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2" t="s">
+      <c r="G22" s="1"/>
+      <c r="H22" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:8" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>1600</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:8" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>1000</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2" t="s">
+      <c r="G24" s="1"/>
+      <c r="H24" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:8" s="2" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>1200</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2" t="s">
+      <c r="G25" s="1"/>
+      <c r="H25" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:8" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>1700</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2" t="s">
+      <c r="G26" s="1"/>
+      <c r="H26" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:8" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>1200</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>1500</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="G28" s="1"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>1500</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2" t="s">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="G29" s="1"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>900</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2" t="s">
+      <c r="G30" s="1"/>
+      <c r="H30" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>1100</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H31" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>1600</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H32" s="3" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="4" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B33" s="1">
+        <v>800</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="170" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36" s="1">
+        <v>900</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1300</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1600</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>